<commit_message>
Notebook file for mtcars
</commit_message>
<xml_diff>
--- a/Regression Model/mtcars.xlsx
+++ b/Regression Model/mtcars.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mtcars" sheetId="1" r:id="rId1"/>
@@ -701,11 +701,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980210176"/>
-        <c:axId val="-1980206416"/>
+        <c:axId val="-2058886208"/>
+        <c:axId val="-1970041696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980210176"/>
+        <c:axId val="-2058886208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,12 +803,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980206416"/>
+        <c:crossAx val="-1970041696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980206416"/>
+        <c:axId val="-1970041696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980210176"/>
+        <c:crossAx val="-2058886208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1215,11 +1215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097259456"/>
-        <c:axId val="-2097256336"/>
+        <c:axId val="-1969708112"/>
+        <c:axId val="-1969704992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097259456"/>
+        <c:axId val="-1969708112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,12 +1317,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097256336"/>
+        <c:crossAx val="-1969704992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097256336"/>
+        <c:axId val="-1969704992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,7 +1414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097259456"/>
+        <c:crossAx val="-1969708112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1723,11 +1723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098136448"/>
-        <c:axId val="-2098134016"/>
+        <c:axId val="-1969683776"/>
+        <c:axId val="-1969680656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098136448"/>
+        <c:axId val="-1969683776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,12 +1825,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098134016"/>
+        <c:crossAx val="-1969680656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098134016"/>
+        <c:axId val="-1969680656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +1922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098136448"/>
+        <c:crossAx val="-1969683776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2231,11 +2231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097737664"/>
-        <c:axId val="-2097719472"/>
+        <c:axId val="-1969659488"/>
+        <c:axId val="-1969656368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097737664"/>
+        <c:axId val="-1969659488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2333,12 +2333,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097719472"/>
+        <c:crossAx val="-1969656368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097719472"/>
+        <c:axId val="-1969656368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,7 +2430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097737664"/>
+        <c:crossAx val="-1969659488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2739,11 +2739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097829856"/>
-        <c:axId val="-2097473232"/>
+        <c:axId val="-1969635152"/>
+        <c:axId val="-1969632032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097829856"/>
+        <c:axId val="-1969635152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,12 +2841,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097473232"/>
+        <c:crossAx val="-1969632032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097473232"/>
+        <c:axId val="-1969632032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2938,7 +2938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097829856"/>
+        <c:crossAx val="-1969635152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3212,11 +3212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095975712"/>
-        <c:axId val="-2097821824"/>
+        <c:axId val="-1969615168"/>
+        <c:axId val="-1969612048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095975712"/>
+        <c:axId val="-1969615168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3314,12 +3314,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097821824"/>
+        <c:crossAx val="-1969612048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097821824"/>
+        <c:axId val="-1969612048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,7 +3411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095975712"/>
+        <c:crossAx val="-1969615168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3685,11 +3685,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097800256"/>
-        <c:axId val="-2097797136"/>
+        <c:axId val="-1969590896"/>
+        <c:axId val="-1969587776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097800256"/>
+        <c:axId val="-1969590896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3787,12 +3787,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097797136"/>
+        <c:crossAx val="-1969587776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097797136"/>
+        <c:axId val="-1969587776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3884,7 +3884,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097800256"/>
+        <c:crossAx val="-1969590896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4158,11 +4158,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097775984"/>
-        <c:axId val="-2097772864"/>
+        <c:axId val="-1969566624"/>
+        <c:axId val="-1969563504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097775984"/>
+        <c:axId val="-1969566624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4260,12 +4260,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097772864"/>
+        <c:crossAx val="-1969563504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097772864"/>
+        <c:axId val="-1969563504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097775984"/>
+        <c:crossAx val="-1969566624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4970,11 +4970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097746928"/>
-        <c:axId val="-2097743808"/>
+        <c:axId val="-1969537760"/>
+        <c:axId val="-1969534640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097746928"/>
+        <c:axId val="-1969537760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5072,12 +5072,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097743808"/>
+        <c:crossAx val="-1969534640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097743808"/>
+        <c:axId val="-1969534640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5169,7 +5169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097746928"/>
+        <c:crossAx val="-1969537760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5716,11 +5716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980726128"/>
-        <c:axId val="-1980574688"/>
+        <c:axId val="-1969507760"/>
+        <c:axId val="-1969504640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980726128"/>
+        <c:axId val="-1969507760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5818,12 +5818,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980574688"/>
+        <c:crossAx val="-1969504640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980574688"/>
+        <c:axId val="-1969504640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5915,7 +5915,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980726128"/>
+        <c:crossAx val="-1969507760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6450,11 +6450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980635728"/>
-        <c:axId val="-1980579808"/>
+        <c:axId val="-1969478224"/>
+        <c:axId val="-1969475104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980635728"/>
+        <c:axId val="-1969478224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6552,12 +6552,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980579808"/>
+        <c:crossAx val="-1969475104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980579808"/>
+        <c:axId val="-1969475104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6649,7 +6649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980635728"/>
+        <c:crossAx val="-1969478224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7294,11 +7294,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980179872"/>
-        <c:axId val="-1980176112"/>
+        <c:axId val="-2058935376"/>
+        <c:axId val="-1970243664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980179872"/>
+        <c:axId val="-2058935376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7396,12 +7396,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980176112"/>
+        <c:crossAx val="-1970243664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980176112"/>
+        <c:axId val="-1970243664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7493,7 +7493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980179872"/>
+        <c:crossAx val="-2058935376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8027,11 +8027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980544192"/>
-        <c:axId val="-1980540432"/>
+        <c:axId val="-1969448608"/>
+        <c:axId val="-1969445488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980544192"/>
+        <c:axId val="-1969448608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8128,12 +8128,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980540432"/>
+        <c:crossAx val="-1969445488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980540432"/>
+        <c:axId val="-1969445488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8224,7 +8224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980544192"/>
+        <c:crossAx val="-1969448608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8745,11 +8745,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980517904"/>
-        <c:axId val="-1980514560"/>
+        <c:axId val="-1969403760"/>
+        <c:axId val="-1969400640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980517904"/>
+        <c:axId val="-1969403760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8846,12 +8846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980514560"/>
+        <c:crossAx val="-1969400640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980514560"/>
+        <c:axId val="-1969400640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8942,7 +8942,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980517904"/>
+        <c:crossAx val="-1969403760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9463,11 +9463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980488192"/>
-        <c:axId val="-1980484432"/>
+        <c:axId val="-1969374496"/>
+        <c:axId val="-1969371376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980488192"/>
+        <c:axId val="-1969374496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9564,12 +9564,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980484432"/>
+        <c:crossAx val="-1969371376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980484432"/>
+        <c:axId val="-1969371376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9660,7 +9660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980488192"/>
+        <c:crossAx val="-1969374496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10181,11 +10181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980457824"/>
-        <c:axId val="-1980454064"/>
+        <c:axId val="-1969345232"/>
+        <c:axId val="-1969342112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980457824"/>
+        <c:axId val="-1969345232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10282,12 +10282,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980454064"/>
+        <c:crossAx val="-1969342112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980454064"/>
+        <c:axId val="-1969342112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10378,7 +10378,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980457824"/>
+        <c:crossAx val="-1969345232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10829,11 +10829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980426400"/>
-        <c:axId val="-1980422640"/>
+        <c:axId val="-1969315824"/>
+        <c:axId val="-1969312704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980426400"/>
+        <c:axId val="-1969315824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10894,6 +10894,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10930,12 +10931,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980422640"/>
+        <c:crossAx val="-1969312704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980422640"/>
+        <c:axId val="-1969312704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11026,7 +11027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980426400"/>
+        <c:crossAx val="-1969315824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11477,11 +11478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980396688"/>
-        <c:axId val="-1980392928"/>
+        <c:axId val="-1969286960"/>
+        <c:axId val="-1969283840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980396688"/>
+        <c:axId val="-1969286960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11578,12 +11579,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980392928"/>
+        <c:crossAx val="-1969283840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980392928"/>
+        <c:axId val="-1969283840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11674,7 +11675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980396688"/>
+        <c:crossAx val="-1969286960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12125,11 +12126,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980367344"/>
-        <c:axId val="-1980363584"/>
+        <c:axId val="-1969258192"/>
+        <c:axId val="-1969255072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980367344"/>
+        <c:axId val="-1969258192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12190,6 +12191,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12226,12 +12228,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980363584"/>
+        <c:crossAx val="-1969255072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980363584"/>
+        <c:axId val="-1969255072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12322,7 +12324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980367344"/>
+        <c:crossAx val="-1969258192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12723,11 +12725,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980326704"/>
-        <c:axId val="-1980322944"/>
+        <c:axId val="-1969431376"/>
+        <c:axId val="-1969428256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980326704"/>
+        <c:axId val="-1969431376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12825,12 +12827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980322944"/>
+        <c:crossAx val="-1969428256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980322944"/>
+        <c:axId val="-1969428256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12922,7 +12924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980326704"/>
+        <c:crossAx val="-1969431376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13207,11 +13209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980301712"/>
-        <c:axId val="-1980297952"/>
+        <c:axId val="-1969875616"/>
+        <c:axId val="-1969872496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980301712"/>
+        <c:axId val="-1969875616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13309,12 +13311,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980297952"/>
+        <c:crossAx val="-1969872496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980297952"/>
+        <c:axId val="-1969872496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13406,7 +13408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980301712"/>
+        <c:crossAx val="-1969875616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14019,11 +14021,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980271328"/>
-        <c:axId val="-1980267568"/>
+        <c:axId val="-1969846160"/>
+        <c:axId val="-1969843040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980271328"/>
+        <c:axId val="-1969846160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14121,12 +14123,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980267568"/>
+        <c:crossAx val="-1969843040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980267568"/>
+        <c:axId val="-1969843040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14218,7 +14220,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980271328"/>
+        <c:crossAx val="-1969846160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14371,7 +14373,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.122241469816273"/>
+          <c:y val="0.226158536585366"/>
+          <c:w val="0.832732889158086"/>
+          <c:h val="0.299582773189937"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -14693,11 +14705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1980241936"/>
-        <c:axId val="-1980238176"/>
+        <c:axId val="-1969817776"/>
+        <c:axId val="-1969814656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1980241936"/>
+        <c:axId val="-1969817776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14795,12 +14807,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980238176"/>
+        <c:crossAx val="-1969814656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1980238176"/>
+        <c:axId val="-1969814656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14892,7 +14904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980241936"/>
+        <c:crossAx val="-1969817776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15294,11 +15306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2097715712"/>
-        <c:axId val="2095202016"/>
+        <c:axId val="-1969784064"/>
+        <c:axId val="-1969780944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2097715712"/>
+        <c:axId val="-1969784064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15396,12 +15408,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095202016"/>
+        <c:crossAx val="-1969780944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095202016"/>
+        <c:axId val="-1969780944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15493,7 +15505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097715712"/>
+        <c:crossAx val="-1969784064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15814,11 +15826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098021168"/>
-        <c:axId val="-2097982512"/>
+        <c:axId val="-1969759536"/>
+        <c:axId val="-1969756416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098021168"/>
+        <c:axId val="-1969759536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15916,12 +15928,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097982512"/>
+        <c:crossAx val="-1969756416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2097982512"/>
+        <c:axId val="-1969756416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16013,7 +16025,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098021168"/>
+        <c:crossAx val="-1969759536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16328,11 +16340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098096720"/>
-        <c:axId val="-2098059376"/>
+        <c:axId val="-1969735520"/>
+        <c:axId val="-1969732400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098096720"/>
+        <c:axId val="-1969735520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16430,12 +16442,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098059376"/>
+        <c:crossAx val="-1969732400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098059376"/>
+        <c:axId val="-1969732400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16527,7 +16539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098096720"/>
+        <c:crossAx val="-1969735520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -30769,8 +30781,8 @@
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -30793,16 +30805,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30823,16 +30835,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30853,16 +30865,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -31775,7 +31787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -33052,13 +33064,18 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -33751,10 +33768,18 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I57"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -34474,11 +34499,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>